<commit_message>
Add version change log
</commit_message>
<xml_diff>
--- a/files/Sport-UI-Type.xlsx
+++ b/files/Sport-UI-Type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kilnn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android\Workspace\FitCloudPro-SDK-Android\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748FAAB9-5370-410C-931B-62904F09D9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191FEE1E-CA0E-406E-81BC-CD094A152081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="843" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="843" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="运动模式编号" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="608">
   <si>
     <t>0x04</t>
   </si>
@@ -1506,6 +1506,645 @@
     </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
+  <si>
+    <t>Spinning</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>动感单车</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x74</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01D1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01D5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x75</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>肚皮舞</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BellyDance</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SquareDance</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>广场舞</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01D9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x76</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>交际舞</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BallroomDance</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01DD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x77</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>尊巴</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zumba</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01E1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x78</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stepper</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>踏步机</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jazz</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>爵士舞</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01E5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01E9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x79</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClimbingMachine</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>爬楼机</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01ED</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Croquet</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>门球</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01F1</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01F5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01F9</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01FD</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>WaterPolo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>水球</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>WallBall</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>墙球</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>台球</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Billiards</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sepaktakraw</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>藤球</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0201</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>杠铃</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0205</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>拉伸</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stretching</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>自由体操</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0209</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FloorExercise</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x020D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Barbell</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>WeightLifting</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>举重</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0211</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HardDrawn</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0215</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>硬拉</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>波比跳</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0219</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BobbyJump</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>开合跳</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x021D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>JumpingJack</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>upper_limb_training</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>lower_limb_training</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>上肢训练</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>下肢训练</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0221</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0225</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0229</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>背部训练</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>BackTraining</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>沙滩车</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x022D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATV</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑翔伞</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Flying kites</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>放风筝</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0235</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0231</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Paraglider</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>TugOfWar</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0239</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>拔河</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁人三项</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x023D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Triathlon</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Snowmobile</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪地摩托</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0241</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0245</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0249</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x024D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0251</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0255</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0259</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x025D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0261</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0265</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0269</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x026D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪车</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>雪橇</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>滑雪板</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>越野滑雪</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>室内滑冰</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡巴迪</t>
+  </si>
+  <si>
+    <t>泰拳</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>踢拳</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛车</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>室内健身</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>户外足球</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outdoor Football</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indoor Fitness</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Racing Car</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kickboxing</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Muay Thai</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kabaddi</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indoor Skating</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cross Country Skiing</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ski Board</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sled</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bobsleigh</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x7F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x80</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x81</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x82</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x83</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x84</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x85</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x86</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x87</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x88</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x89</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8E</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x8F</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x90</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x91</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x92</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x93</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x94</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x95</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x96</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x97</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x98</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x99</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x9A</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x9B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1580,7 +2219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1593,8 +2232,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1730,13 +2375,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1782,10 +2447,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1794,19 +2465,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2113,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="I152" sqref="I152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2132,38 +2824,38 @@
       <c r="A1" s="21" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6" spans="1:5" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
@@ -2172,13 +2864,13 @@
       <c r="B6" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="15" t="s">
         <v>416</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>415</v>
       </c>
-      <c r="E6" s="18"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -2190,10 +2882,10 @@
       <c r="C7" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="19" t="s">
         <v>418</v>
       </c>
-      <c r="E7" s="18"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
@@ -2205,10 +2897,10 @@
       <c r="C8" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -2220,10 +2912,10 @@
       <c r="C9" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -2235,10 +2927,10 @@
       <c r="C10" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="19" t="s">
         <v>429</v>
       </c>
-      <c r="E10" s="18"/>
+      <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2250,10 +2942,10 @@
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -2265,10 +2957,10 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -2280,10 +2972,10 @@
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2295,10 +2987,10 @@
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -2310,10 +3002,10 @@
       <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -2325,10 +3017,10 @@
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -2340,10 +3032,10 @@
       <c r="C17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="17"/>
     </row>
     <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -2355,10 +3047,10 @@
       <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="16"/>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -2370,10 +3062,10 @@
       <c r="C19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="17"/>
     </row>
     <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -2385,10 +3077,10 @@
       <c r="C20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -2400,10 +3092,10 @@
       <c r="C21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -2415,10 +3107,10 @@
       <c r="C22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -2430,10 +3122,10 @@
       <c r="C23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -2445,10 +3137,10 @@
       <c r="C24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
@@ -2460,10 +3152,10 @@
       <c r="C25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="16"/>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -2475,10 +3167,10 @@
       <c r="C26" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="16"/>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
@@ -2490,10 +3182,10 @@
       <c r="C27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="16"/>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
@@ -2505,10 +3197,10 @@
       <c r="C28" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="16"/>
+      <c r="E28" s="17"/>
     </row>
     <row r="29" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -2520,10 +3212,10 @@
       <c r="C29" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="16"/>
+      <c r="E29" s="17"/>
     </row>
     <row r="30" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
@@ -2535,10 +3227,10 @@
       <c r="C30" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="16"/>
+      <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -2550,10 +3242,10 @@
       <c r="C31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="16"/>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
@@ -2565,10 +3257,10 @@
       <c r="C32" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="16"/>
+      <c r="E32" s="17"/>
     </row>
     <row r="33" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -2580,10 +3272,10 @@
       <c r="C33" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="16"/>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -2595,10 +3287,10 @@
       <c r="C34" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="16"/>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -2610,10 +3302,10 @@
       <c r="C35" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="17"/>
     </row>
     <row r="36" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
@@ -2625,10 +3317,10 @@
       <c r="C36" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="16"/>
+      <c r="E36" s="17"/>
     </row>
     <row r="37" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -2640,10 +3332,10 @@
       <c r="C37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E37" s="16"/>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
@@ -2655,10 +3347,10 @@
       <c r="C38" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="16"/>
+      <c r="E38" s="17"/>
     </row>
     <row r="39" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
@@ -2670,10 +3362,10 @@
       <c r="C39" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="20"/>
+      <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -2685,10 +3377,10 @@
       <c r="C40" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="20"/>
+      <c r="E40" s="18"/>
     </row>
     <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
@@ -2700,10 +3392,10 @@
       <c r="C41" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D41" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="20"/>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -2715,10 +3407,10 @@
       <c r="C42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D42" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="20"/>
+      <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -2730,10 +3422,10 @@
       <c r="C43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D43" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -2745,10 +3437,10 @@
       <c r="C44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="20"/>
+      <c r="E44" s="18"/>
     </row>
     <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -2760,10 +3452,10 @@
       <c r="C45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E45" s="20"/>
+      <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
@@ -2775,10 +3467,10 @@
       <c r="C46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D46" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="20"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
@@ -2790,10 +3482,10 @@
       <c r="C47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="20"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
@@ -2805,10 +3497,10 @@
       <c r="C48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="20"/>
+      <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
@@ -2820,10 +3512,10 @@
       <c r="C49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="16" t="s">
         <v>138</v>
       </c>
-      <c r="E49" s="16"/>
+      <c r="E49" s="17"/>
     </row>
     <row r="50" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
@@ -2835,10 +3527,10 @@
       <c r="C50" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="E50" s="16"/>
+      <c r="E50" s="17"/>
     </row>
     <row r="51" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
@@ -2850,10 +3542,10 @@
       <c r="C51" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="E51" s="16"/>
+      <c r="E51" s="17"/>
     </row>
     <row r="52" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
@@ -2865,10 +3557,10 @@
       <c r="C52" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="E52" s="16"/>
+      <c r="E52" s="17"/>
     </row>
     <row r="53" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
@@ -2880,10 +3572,10 @@
       <c r="C53" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="16"/>
+      <c r="E53" s="17"/>
     </row>
     <row r="54" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
@@ -2895,10 +3587,10 @@
       <c r="C54" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="E54" s="16"/>
+      <c r="E54" s="17"/>
     </row>
     <row r="55" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
@@ -2910,10 +3602,10 @@
       <c r="C55" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E55" s="16"/>
+      <c r="E55" s="17"/>
     </row>
     <row r="56" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
@@ -2925,10 +3617,10 @@
       <c r="C56" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E56" s="16"/>
+      <c r="E56" s="17"/>
     </row>
     <row r="57" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
@@ -2940,10 +3632,10 @@
       <c r="C57" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="16"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
@@ -2955,10 +3647,10 @@
       <c r="C58" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="16"/>
+      <c r="E58" s="17"/>
     </row>
     <row r="59" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
@@ -2970,10 +3662,10 @@
       <c r="C59" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="16"/>
+      <c r="E59" s="17"/>
     </row>
     <row r="60" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
@@ -2985,10 +3677,10 @@
       <c r="C60" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E60" s="16"/>
+      <c r="E60" s="17"/>
     </row>
     <row r="61" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
@@ -3000,10 +3692,10 @@
       <c r="C61" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E61" s="16"/>
+      <c r="E61" s="17"/>
     </row>
     <row r="62" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
@@ -3015,10 +3707,10 @@
       <c r="C62" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E62" s="16"/>
+      <c r="E62" s="17"/>
     </row>
     <row r="63" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
@@ -3030,10 +3722,10 @@
       <c r="C63" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E63" s="16"/>
+      <c r="E63" s="17"/>
     </row>
     <row r="64" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
@@ -3045,10 +3737,10 @@
       <c r="C64" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E64" s="16"/>
+      <c r="E64" s="17"/>
     </row>
     <row r="65" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
@@ -3060,10 +3752,10 @@
       <c r="C65" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="E65" s="16"/>
+      <c r="E65" s="17"/>
     </row>
     <row r="66" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
@@ -3075,10 +3767,10 @@
       <c r="C66" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="16"/>
+      <c r="E66" s="17"/>
     </row>
     <row r="67" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
@@ -3090,10 +3782,10 @@
       <c r="C67" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="E67" s="16"/>
+      <c r="E67" s="17"/>
     </row>
     <row r="68" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
@@ -3105,10 +3797,10 @@
       <c r="C68" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="16" t="s">
         <v>185</v>
       </c>
-      <c r="E68" s="16"/>
+      <c r="E68" s="17"/>
     </row>
     <row r="69" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
@@ -3120,10 +3812,10 @@
       <c r="C69" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="16" t="s">
         <v>188</v>
       </c>
-      <c r="E69" s="16"/>
+      <c r="E69" s="17"/>
     </row>
     <row r="70" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
@@ -3135,10 +3827,10 @@
       <c r="C70" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E70" s="16"/>
+      <c r="E70" s="17"/>
     </row>
     <row r="71" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
@@ -3150,10 +3842,10 @@
       <c r="C71" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D71" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E71" s="16"/>
+      <c r="E71" s="17"/>
     </row>
     <row r="72" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
@@ -3165,10 +3857,10 @@
       <c r="C72" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D72" s="15" t="s">
+      <c r="D72" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E72" s="16"/>
+      <c r="E72" s="17"/>
     </row>
     <row r="73" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
@@ -3180,10 +3872,10 @@
       <c r="C73" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E73" s="16"/>
+      <c r="E73" s="17"/>
     </row>
     <row r="74" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
@@ -3195,10 +3887,10 @@
       <c r="C74" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E74" s="16"/>
+      <c r="E74" s="17"/>
     </row>
     <row r="75" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
@@ -3210,10 +3902,10 @@
       <c r="C75" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E75" s="16"/>
+      <c r="E75" s="17"/>
     </row>
     <row r="76" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
@@ -3225,10 +3917,10 @@
       <c r="C76" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="D76" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E76" s="16"/>
+      <c r="E76" s="17"/>
     </row>
     <row r="77" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
@@ -3240,10 +3932,10 @@
       <c r="C77" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D77" s="15" t="s">
+      <c r="D77" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E77" s="16"/>
+      <c r="E77" s="17"/>
     </row>
     <row r="78" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
@@ -3255,10 +3947,10 @@
       <c r="C78" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D78" s="15" t="s">
+      <c r="D78" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E78" s="16"/>
+      <c r="E78" s="17"/>
     </row>
     <row r="79" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
@@ -3270,10 +3962,10 @@
       <c r="C79" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E79" s="16"/>
+      <c r="E79" s="17"/>
     </row>
     <row r="80" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
@@ -3285,10 +3977,10 @@
       <c r="C80" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E80" s="16"/>
+      <c r="E80" s="17"/>
     </row>
     <row r="81" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
@@ -3300,10 +3992,10 @@
       <c r="C81" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="E81" s="16"/>
+      <c r="E81" s="17"/>
     </row>
     <row r="82" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
@@ -3315,10 +4007,10 @@
       <c r="C82" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D82" s="15" t="s">
+      <c r="D82" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="E82" s="16"/>
+      <c r="E82" s="17"/>
     </row>
     <row r="83" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
@@ -3330,10 +4022,10 @@
       <c r="C83" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="E83" s="16"/>
+      <c r="E83" s="17"/>
     </row>
     <row r="84" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
@@ -3345,10 +4037,10 @@
       <c r="C84" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D84" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="E84" s="16"/>
+      <c r="E84" s="17"/>
     </row>
     <row r="85" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
@@ -3360,10 +4052,10 @@
       <c r="C85" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="E85" s="16"/>
+      <c r="E85" s="17"/>
     </row>
     <row r="86" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
@@ -3375,10 +4067,10 @@
       <c r="C86" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="D86" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="E86" s="16"/>
+      <c r="E86" s="17"/>
     </row>
     <row r="87" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
@@ -3390,10 +4082,10 @@
       <c r="C87" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E87" s="16"/>
+      <c r="E87" s="17"/>
     </row>
     <row r="88" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
@@ -3405,10 +4097,10 @@
       <c r="C88" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="D88" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E88" s="16"/>
+      <c r="E88" s="17"/>
     </row>
     <row r="89" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
@@ -3420,10 +4112,10 @@
       <c r="C89" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D89" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E89" s="16"/>
+      <c r="E89" s="17"/>
     </row>
     <row r="90" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
@@ -3435,10 +4127,10 @@
       <c r="C90" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D90" s="15" t="s">
+      <c r="D90" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="E90" s="16"/>
+      <c r="E90" s="17"/>
     </row>
     <row r="91" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
@@ -3450,10 +4142,10 @@
       <c r="C91" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D91" s="15" t="s">
+      <c r="D91" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E91" s="16"/>
+      <c r="E91" s="17"/>
     </row>
     <row r="92" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
@@ -3465,10 +4157,10 @@
       <c r="C92" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="16" t="s">
         <v>241</v>
       </c>
-      <c r="E92" s="16"/>
+      <c r="E92" s="17"/>
     </row>
     <row r="93" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
@@ -3480,10 +4172,10 @@
       <c r="C93" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D93" s="15" t="s">
+      <c r="D93" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="E93" s="16"/>
+      <c r="E93" s="17"/>
     </row>
     <row r="94" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
@@ -3495,10 +4187,10 @@
       <c r="C94" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D94" s="15" t="s">
+      <c r="D94" s="16" t="s">
         <v>247</v>
       </c>
-      <c r="E94" s="16"/>
+      <c r="E94" s="17"/>
     </row>
     <row r="95" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
@@ -3510,10 +4202,10 @@
       <c r="C95" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D95" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="E95" s="16"/>
+      <c r="E95" s="17"/>
     </row>
     <row r="96" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
@@ -3525,10 +4217,10 @@
       <c r="C96" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D96" s="15" t="s">
+      <c r="D96" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E96" s="16"/>
+      <c r="E96" s="17"/>
     </row>
     <row r="97" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
@@ -3540,10 +4232,10 @@
       <c r="C97" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D97" s="15" t="s">
+      <c r="D97" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="E97" s="16"/>
+      <c r="E97" s="17"/>
     </row>
     <row r="98" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
@@ -3555,10 +4247,10 @@
       <c r="C98" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D98" s="15" t="s">
+      <c r="D98" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="E98" s="16"/>
+      <c r="E98" s="17"/>
     </row>
     <row r="99" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
@@ -3570,10 +4262,10 @@
       <c r="C99" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D99" s="15" t="s">
+      <c r="D99" s="16" t="s">
         <v>261</v>
       </c>
-      <c r="E99" s="16"/>
+      <c r="E99" s="17"/>
     </row>
     <row r="100" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
@@ -3585,10 +4277,10 @@
       <c r="C100" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D100" s="15" t="s">
+      <c r="D100" s="16" t="s">
         <v>264</v>
       </c>
-      <c r="E100" s="16"/>
+      <c r="E100" s="17"/>
     </row>
     <row r="101" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
@@ -3600,10 +4292,10 @@
       <c r="C101" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D101" s="15" t="s">
+      <c r="D101" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="E101" s="16"/>
+      <c r="E101" s="17"/>
     </row>
     <row r="102" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
@@ -3615,10 +4307,10 @@
       <c r="C102" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="D102" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="E102" s="16"/>
+      <c r="E102" s="17"/>
     </row>
     <row r="103" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
@@ -3630,10 +4322,10 @@
       <c r="C103" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D103" s="15" t="s">
+      <c r="D103" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E103" s="16"/>
+      <c r="E103" s="17"/>
     </row>
     <row r="104" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
@@ -3645,10 +4337,10 @@
       <c r="C104" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D104" s="15" t="s">
+      <c r="D104" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E104" s="16"/>
+      <c r="E104" s="17"/>
     </row>
     <row r="105" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
@@ -3660,10 +4352,10 @@
       <c r="C105" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D105" s="15" t="s">
+      <c r="D105" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E105" s="16"/>
+      <c r="E105" s="17"/>
     </row>
     <row r="106" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
@@ -3675,10 +4367,10 @@
       <c r="C106" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D106" s="15" t="s">
+      <c r="D106" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E106" s="16"/>
+      <c r="E106" s="17"/>
     </row>
     <row r="107" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
@@ -3690,10 +4382,10 @@
       <c r="C107" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D107" s="15" t="s">
+      <c r="D107" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="E107" s="16"/>
+      <c r="E107" s="17"/>
     </row>
     <row r="108" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
@@ -3705,10 +4397,10 @@
       <c r="C108" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D108" s="15" t="s">
+      <c r="D108" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E108" s="16"/>
+      <c r="E108" s="17"/>
     </row>
     <row r="109" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
@@ -3720,10 +4412,10 @@
       <c r="C109" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D109" s="15" t="s">
+      <c r="D109" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E109" s="16"/>
+      <c r="E109" s="17"/>
     </row>
     <row r="110" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12" t="s">
@@ -3735,10 +4427,10 @@
       <c r="C110" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D110" s="15" t="s">
+      <c r="D110" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E110" s="16"/>
+      <c r="E110" s="17"/>
     </row>
     <row r="111" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
@@ -3750,10 +4442,10 @@
       <c r="C111" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D111" s="15" t="s">
+      <c r="D111" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E111" s="16"/>
+      <c r="E111" s="17"/>
     </row>
     <row r="112" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
@@ -3765,10 +4457,10 @@
       <c r="C112" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D112" s="15" t="s">
+      <c r="D112" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E112" s="16"/>
+      <c r="E112" s="17"/>
     </row>
     <row r="113" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
@@ -3780,10 +4472,10 @@
       <c r="C113" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D113" s="15" t="s">
+      <c r="D113" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E113" s="16"/>
+      <c r="E113" s="17"/>
     </row>
     <row r="114" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12" t="s">
@@ -3795,10 +4487,10 @@
       <c r="C114" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D114" s="15" t="s">
+      <c r="D114" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="E114" s="16"/>
+      <c r="E114" s="17"/>
     </row>
     <row r="115" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
@@ -3810,10 +4502,10 @@
       <c r="C115" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D115" s="15" t="s">
+      <c r="D115" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="E115" s="16"/>
+      <c r="E115" s="17"/>
     </row>
     <row r="116" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
@@ -3825,10 +4517,10 @@
       <c r="C116" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D116" s="15" t="s">
+      <c r="D116" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="E116" s="16"/>
+      <c r="E116" s="17"/>
     </row>
     <row r="117" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12" t="s">
@@ -3840,10 +4532,10 @@
       <c r="C117" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D117" s="15" t="s">
+      <c r="D117" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="E117" s="16"/>
+      <c r="E117" s="17"/>
     </row>
     <row r="118" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
@@ -3855,10 +4547,10 @@
       <c r="C118" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D118" s="15" t="s">
+      <c r="D118" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E118" s="16"/>
+      <c r="E118" s="17"/>
     </row>
     <row r="119" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
@@ -3870,10 +4562,10 @@
       <c r="C119" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D119" s="15" t="s">
+      <c r="D119" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E119" s="16"/>
+      <c r="E119" s="17"/>
     </row>
     <row r="120" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
@@ -3885,10 +4577,10 @@
       <c r="C120" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D120" s="15" t="s">
+      <c r="D120" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="E120" s="16"/>
+      <c r="E120" s="17"/>
     </row>
     <row r="121" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
@@ -3900,12 +4592,12 @@
       <c r="C121" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D121" s="15" t="s">
+      <c r="D121" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E121" s="16"/>
-    </row>
-    <row r="122" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="E121" s="17"/>
+    </row>
+    <row r="122" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12" t="s">
         <v>414</v>
       </c>
@@ -3915,23 +4607,991 @@
       <c r="C122" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D122" s="15" t="s">
+      <c r="D122" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E122" s="16"/>
+      <c r="E122" s="17"/>
+    </row>
+    <row r="123" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="B123" s="32" t="s">
+        <v>449</v>
+      </c>
+      <c r="C123" s="32" t="s">
+        <v>451</v>
+      </c>
+      <c r="D123" s="28" t="s">
+        <v>450</v>
+      </c>
+      <c r="E123" s="29"/>
+    </row>
+    <row r="124" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="26" t="s">
+        <v>455</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="C124" s="32" t="s">
+        <v>452</v>
+      </c>
+      <c r="D124" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="E124" s="29"/>
+    </row>
+    <row r="125" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="26" t="s">
+        <v>456</v>
+      </c>
+      <c r="B125" s="32" t="s">
+        <v>457</v>
+      </c>
+      <c r="C125" s="32" t="s">
+        <v>458</v>
+      </c>
+      <c r="D125" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="E125" s="29"/>
+    </row>
+    <row r="126" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="B126" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="C126" s="32" t="s">
+        <v>462</v>
+      </c>
+      <c r="D126" s="28" t="s">
+        <v>463</v>
+      </c>
+      <c r="E126" s="29"/>
+    </row>
+    <row r="127" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="B127" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="C127" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="D127" s="28" t="s">
+        <v>467</v>
+      </c>
+      <c r="E127" s="29"/>
+    </row>
+    <row r="128" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="30" t="s">
+        <v>470</v>
+      </c>
+      <c r="B128" s="30" t="s">
+        <v>471</v>
+      </c>
+      <c r="C128" s="31" t="s">
+        <v>472</v>
+      </c>
+      <c r="D128" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="E128" s="29"/>
+    </row>
+    <row r="129" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="26" t="s">
+        <v>468</v>
+      </c>
+      <c r="B129" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="C129" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="D129" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="E129" s="29"/>
+    </row>
+    <row r="130" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="B130" s="26" t="s">
+        <v>477</v>
+      </c>
+      <c r="C130" s="31" t="s">
+        <v>478</v>
+      </c>
+      <c r="D130" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="E130" s="29"/>
+    </row>
+    <row r="131" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="26" t="s">
+        <v>480</v>
+      </c>
+      <c r="B131" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>482</v>
+      </c>
+      <c r="D131" s="28" t="s">
+        <v>576</v>
+      </c>
+      <c r="E131" s="29"/>
+    </row>
+    <row r="132" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="26" t="s">
+        <v>486</v>
+      </c>
+      <c r="B132" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="C132" s="27" t="s">
+        <v>483</v>
+      </c>
+      <c r="D132" s="28" t="s">
+        <v>577</v>
+      </c>
+      <c r="E132" s="29"/>
+    </row>
+    <row r="133" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="B133" s="26" t="s">
+        <v>489</v>
+      </c>
+      <c r="C133" s="31" t="s">
+        <v>484</v>
+      </c>
+      <c r="D133" s="28" t="s">
+        <v>578</v>
+      </c>
+      <c r="E133" s="29"/>
+    </row>
+    <row r="134" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="26" t="s">
+        <v>491</v>
+      </c>
+      <c r="B134" s="26" t="s">
+        <v>490</v>
+      </c>
+      <c r="C134" s="31" t="s">
+        <v>485</v>
+      </c>
+      <c r="D134" s="28" t="s">
+        <v>579</v>
+      </c>
+      <c r="E134" s="29"/>
+    </row>
+    <row r="135" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="26" t="s">
+        <v>492</v>
+      </c>
+      <c r="B135" s="26" t="s">
+        <v>493</v>
+      </c>
+      <c r="C135" s="27" t="s">
+        <v>494</v>
+      </c>
+      <c r="D135" s="28" t="s">
+        <v>580</v>
+      </c>
+      <c r="E135" s="29"/>
+    </row>
+    <row r="136" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="26" t="s">
+        <v>498</v>
+      </c>
+      <c r="B136" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="C136" s="31" t="s">
+        <v>496</v>
+      </c>
+      <c r="D136" s="28" t="s">
+        <v>581</v>
+      </c>
+      <c r="E136" s="29"/>
+    </row>
+    <row r="137" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="B137" s="26" t="s">
+        <v>499</v>
+      </c>
+      <c r="C137" s="31" t="s">
+        <v>500</v>
+      </c>
+      <c r="D137" s="28" t="s">
+        <v>582</v>
+      </c>
+      <c r="E137" s="29"/>
+    </row>
+    <row r="138" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="B138" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="C138" s="27" t="s">
+        <v>502</v>
+      </c>
+      <c r="D138" s="28" t="s">
+        <v>583</v>
+      </c>
+      <c r="E138" s="29"/>
+    </row>
+    <row r="139" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="B139" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="C139" s="31" t="s">
+        <v>506</v>
+      </c>
+      <c r="D139" s="28" t="s">
+        <v>584</v>
+      </c>
+      <c r="E139" s="29"/>
+    </row>
+    <row r="140" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="26" t="s">
+        <v>507</v>
+      </c>
+      <c r="B140" s="26" t="s">
+        <v>509</v>
+      </c>
+      <c r="C140" s="31" t="s">
+        <v>508</v>
+      </c>
+      <c r="D140" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="E140" s="29"/>
+    </row>
+    <row r="141" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="B141" s="26" t="s">
+        <v>510</v>
+      </c>
+      <c r="C141" s="27" t="s">
+        <v>511</v>
+      </c>
+      <c r="D141" s="28" t="s">
+        <v>586</v>
+      </c>
+      <c r="E141" s="29"/>
+    </row>
+    <row r="142" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="26" t="s">
+        <v>515</v>
+      </c>
+      <c r="B142" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="C142" s="31" t="s">
+        <v>514</v>
+      </c>
+      <c r="D142" s="28" t="s">
+        <v>587</v>
+      </c>
+      <c r="E142" s="29"/>
+    </row>
+    <row r="143" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="26" t="s">
+        <v>516</v>
+      </c>
+      <c r="B143" s="26" t="s">
+        <v>518</v>
+      </c>
+      <c r="C143" s="31" t="s">
+        <v>520</v>
+      </c>
+      <c r="D143" s="28" t="s">
+        <v>588</v>
+      </c>
+      <c r="E143" s="29"/>
+    </row>
+    <row r="144" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="B144" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="C144" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="D144" s="28" t="s">
+        <v>589</v>
+      </c>
+      <c r="E144" s="29"/>
+    </row>
+    <row r="145" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="26" t="s">
+        <v>524</v>
+      </c>
+      <c r="B145" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="C145" s="31" t="s">
+        <v>522</v>
+      </c>
+      <c r="D145" s="28" t="s">
+        <v>590</v>
+      </c>
+      <c r="E145" s="29"/>
+    </row>
+    <row r="146" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="26" t="s">
+        <v>527</v>
+      </c>
+      <c r="B146" s="26" t="s">
+        <v>525</v>
+      </c>
+      <c r="C146" s="31" t="s">
+        <v>526</v>
+      </c>
+      <c r="D146" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="E146" s="29"/>
+    </row>
+    <row r="147" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="26" t="s">
+        <v>533</v>
+      </c>
+      <c r="B147" s="26" t="s">
+        <v>528</v>
+      </c>
+      <c r="C147" s="27" t="s">
+        <v>532</v>
+      </c>
+      <c r="D147" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="E147" s="29"/>
+    </row>
+    <row r="148" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="26" t="s">
+        <v>529</v>
+      </c>
+      <c r="B148" s="26" t="s">
+        <v>530</v>
+      </c>
+      <c r="C148" s="31" t="s">
+        <v>531</v>
+      </c>
+      <c r="D148" s="28" t="s">
+        <v>593</v>
+      </c>
+      <c r="E148" s="29"/>
+    </row>
+    <row r="149" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="26" t="s">
+        <v>534</v>
+      </c>
+      <c r="B149" s="26" t="s">
+        <v>536</v>
+      </c>
+      <c r="C149" s="31" t="s">
+        <v>535</v>
+      </c>
+      <c r="D149" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="E149" s="29"/>
+    </row>
+    <row r="150" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="26" t="s">
+        <v>539</v>
+      </c>
+      <c r="B150" s="26" t="s">
+        <v>537</v>
+      </c>
+      <c r="C150" s="27" t="s">
+        <v>538</v>
+      </c>
+      <c r="D150" s="28" t="s">
+        <v>595</v>
+      </c>
+      <c r="E150" s="29"/>
+    </row>
+    <row r="151" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="26" t="s">
+        <v>540</v>
+      </c>
+      <c r="B151" s="26" t="s">
+        <v>541</v>
+      </c>
+      <c r="C151" s="31" t="s">
+        <v>542</v>
+      </c>
+      <c r="D151" s="28" t="s">
+        <v>596</v>
+      </c>
+      <c r="E151" s="29"/>
+    </row>
+    <row r="152" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="26" t="s">
+        <v>575</v>
+      </c>
+      <c r="B152" s="26" t="s">
+        <v>554</v>
+      </c>
+      <c r="C152" s="31" t="s">
+        <v>543</v>
+      </c>
+      <c r="D152" s="28" t="s">
+        <v>597</v>
+      </c>
+      <c r="E152" s="29"/>
+    </row>
+    <row r="153" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="26" t="s">
+        <v>574</v>
+      </c>
+      <c r="B153" s="26" t="s">
+        <v>555</v>
+      </c>
+      <c r="C153" s="27" t="s">
+        <v>544</v>
+      </c>
+      <c r="D153" s="28" t="s">
+        <v>598</v>
+      </c>
+      <c r="E153" s="29"/>
+    </row>
+    <row r="154" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="26" t="s">
+        <v>573</v>
+      </c>
+      <c r="B154" s="26" t="s">
+        <v>556</v>
+      </c>
+      <c r="C154" s="31" t="s">
+        <v>545</v>
+      </c>
+      <c r="D154" s="28" t="s">
+        <v>599</v>
+      </c>
+      <c r="E154" s="29"/>
+    </row>
+    <row r="155" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="26" t="s">
+        <v>572</v>
+      </c>
+      <c r="B155" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="C155" s="27" t="s">
+        <v>546</v>
+      </c>
+      <c r="D155" s="28" t="s">
+        <v>600</v>
+      </c>
+      <c r="E155" s="29"/>
+    </row>
+    <row r="156" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="26" t="s">
+        <v>571</v>
+      </c>
+      <c r="B156" s="26" t="s">
+        <v>558</v>
+      </c>
+      <c r="C156" s="31" t="s">
+        <v>547</v>
+      </c>
+      <c r="D156" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E156" s="29"/>
+    </row>
+    <row r="157" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="26" t="s">
+        <v>570</v>
+      </c>
+      <c r="B157" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="C157" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="D157" s="28" t="s">
+        <v>602</v>
+      </c>
+      <c r="E157" s="29"/>
+    </row>
+    <row r="158" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="26" t="s">
+        <v>569</v>
+      </c>
+      <c r="B158" s="26" t="s">
+        <v>560</v>
+      </c>
+      <c r="C158" s="31" t="s">
+        <v>549</v>
+      </c>
+      <c r="D158" s="28" t="s">
+        <v>603</v>
+      </c>
+      <c r="E158" s="29"/>
+    </row>
+    <row r="159" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="26" t="s">
+        <v>568</v>
+      </c>
+      <c r="B159" s="26" t="s">
+        <v>561</v>
+      </c>
+      <c r="C159" s="27" t="s">
+        <v>550</v>
+      </c>
+      <c r="D159" s="28" t="s">
+        <v>604</v>
+      </c>
+      <c r="E159" s="29"/>
+    </row>
+    <row r="160" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="B160" s="26" t="s">
+        <v>562</v>
+      </c>
+      <c r="C160" s="31" t="s">
+        <v>551</v>
+      </c>
+      <c r="D160" s="28" t="s">
+        <v>605</v>
+      </c>
+      <c r="E160" s="29"/>
+    </row>
+    <row r="161" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="26" t="s">
+        <v>566</v>
+      </c>
+      <c r="B161" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="C161" s="27" t="s">
+        <v>552</v>
+      </c>
+      <c r="D161" s="28" t="s">
+        <v>606</v>
+      </c>
+      <c r="E161" s="29"/>
+    </row>
+    <row r="162" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="26" t="s">
+        <v>565</v>
+      </c>
+      <c r="B162" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="C162" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="D162" s="28" t="s">
+        <v>607</v>
+      </c>
+      <c r="E162" s="29"/>
+    </row>
+    <row r="163" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="12"/>
+      <c r="B163" s="13"/>
+      <c r="C163" s="25"/>
+      <c r="D163" s="24"/>
+      <c r="E163" s="17"/>
+    </row>
+    <row r="164" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="12"/>
+      <c r="B164" s="13"/>
+      <c r="C164" s="1"/>
+      <c r="D164" s="16"/>
+      <c r="E164" s="17"/>
+    </row>
+    <row r="165" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="12"/>
+      <c r="B165" s="13"/>
+      <c r="C165" s="25"/>
+      <c r="D165" s="24"/>
+      <c r="E165" s="17"/>
+    </row>
+    <row r="166" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A166" s="12"/>
+      <c r="B166" s="13"/>
+      <c r="C166" s="1"/>
+      <c r="D166" s="16"/>
+      <c r="E166" s="17"/>
+    </row>
+    <row r="167" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="12"/>
+      <c r="B167" s="13"/>
+      <c r="C167" s="25"/>
+      <c r="D167" s="24"/>
+      <c r="E167" s="17"/>
+    </row>
+    <row r="168" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A168" s="12"/>
+      <c r="B168" s="13"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="16"/>
+      <c r="E168" s="17"/>
+    </row>
+    <row r="169" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A169" s="12"/>
+      <c r="B169" s="13"/>
+      <c r="C169" s="25"/>
+      <c r="D169" s="24"/>
+      <c r="E169" s="17"/>
+    </row>
+    <row r="170" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A170" s="12"/>
+      <c r="B170" s="13"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="16"/>
+      <c r="E170" s="17"/>
+    </row>
+    <row r="171" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A171" s="12"/>
+      <c r="B171" s="13"/>
+      <c r="C171" s="25"/>
+      <c r="D171" s="24"/>
+      <c r="E171" s="17"/>
+    </row>
+    <row r="172" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A172" s="12"/>
+      <c r="B172" s="13"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="16"/>
+      <c r="E172" s="17"/>
+    </row>
+    <row r="173" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A173" s="12"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="25"/>
+      <c r="D173" s="24"/>
+      <c r="E173" s="17"/>
+    </row>
+    <row r="174" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="12"/>
+      <c r="B174" s="13"/>
+      <c r="C174" s="1"/>
+      <c r="D174" s="16"/>
+      <c r="E174" s="17"/>
+    </row>
+    <row r="175" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A175" s="12"/>
+      <c r="B175" s="13"/>
+      <c r="C175" s="25"/>
+      <c r="D175" s="24"/>
+      <c r="E175" s="17"/>
+    </row>
+    <row r="176" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A176" s="12"/>
+      <c r="B176" s="13"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="16"/>
+      <c r="E176" s="17"/>
+    </row>
+    <row r="177" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="12"/>
+      <c r="B177" s="13"/>
+      <c r="C177" s="25"/>
+      <c r="D177" s="24"/>
+      <c r="E177" s="17"/>
+    </row>
+    <row r="178" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A178" s="12"/>
+      <c r="B178" s="13"/>
+      <c r="C178" s="1"/>
+      <c r="D178" s="16"/>
+      <c r="E178" s="17"/>
+    </row>
+    <row r="179" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A179" s="12"/>
+      <c r="B179" s="13"/>
+      <c r="C179" s="25"/>
+      <c r="D179" s="24"/>
+      <c r="E179" s="17"/>
+    </row>
+    <row r="180" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A180" s="12"/>
+      <c r="B180" s="13"/>
+      <c r="C180" s="1"/>
+      <c r="D180" s="16"/>
+      <c r="E180" s="17"/>
+    </row>
+    <row r="181" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A181" s="12"/>
+      <c r="B181" s="13"/>
+      <c r="C181" s="25"/>
+      <c r="D181" s="24"/>
+      <c r="E181" s="17"/>
+    </row>
+    <row r="182" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A182" s="12"/>
+      <c r="B182" s="13"/>
+      <c r="C182" s="1"/>
+      <c r="D182" s="16"/>
+      <c r="E182" s="17"/>
+    </row>
+    <row r="183" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A183" s="12"/>
+      <c r="B183" s="13"/>
+      <c r="C183" s="25"/>
+      <c r="D183" s="24"/>
+      <c r="E183" s="17"/>
+    </row>
+    <row r="184" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="12"/>
+      <c r="B184" s="13"/>
+      <c r="C184" s="1"/>
+      <c r="D184" s="16"/>
+      <c r="E184" s="17"/>
+    </row>
+    <row r="185" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A185" s="12"/>
+      <c r="B185" s="13"/>
+      <c r="C185" s="25"/>
+      <c r="D185" s="24"/>
+      <c r="E185" s="17"/>
+    </row>
+    <row r="186" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A186" s="12"/>
+      <c r="B186" s="13"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="16"/>
+      <c r="E186" s="17"/>
+    </row>
+    <row r="187" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A187" s="12"/>
+      <c r="B187" s="13"/>
+      <c r="C187" s="25"/>
+      <c r="D187" s="24"/>
+      <c r="E187" s="17"/>
+    </row>
+    <row r="188" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="12"/>
+      <c r="B188" s="13"/>
+      <c r="C188" s="1"/>
+      <c r="D188" s="16"/>
+      <c r="E188" s="17"/>
+    </row>
+    <row r="189" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A189" s="12"/>
+      <c r="B189" s="13"/>
+      <c r="C189" s="25"/>
+      <c r="D189" s="24"/>
+      <c r="E189" s="17"/>
+    </row>
+    <row r="190" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A190" s="12"/>
+      <c r="B190" s="13"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="16"/>
+      <c r="E190" s="17"/>
+    </row>
+    <row r="191" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A191" s="12"/>
+      <c r="B191" s="13"/>
+      <c r="C191" s="25"/>
+      <c r="D191" s="24"/>
+      <c r="E191" s="17"/>
+    </row>
+    <row r="192" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A192" s="12"/>
+      <c r="B192" s="13"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="16"/>
+      <c r="E192" s="17"/>
+    </row>
+    <row r="193" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A193" s="12"/>
+      <c r="B193" s="13"/>
+      <c r="C193" s="25"/>
+      <c r="D193" s="24"/>
+      <c r="E193" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
+  <mergeCells count="189">
+    <mergeCell ref="D186:E186"/>
+    <mergeCell ref="D187:E187"/>
+    <mergeCell ref="D188:E188"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="D190:E190"/>
+    <mergeCell ref="D191:E191"/>
+    <mergeCell ref="D192:E192"/>
+    <mergeCell ref="D193:E193"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
+    <mergeCell ref="D179:E179"/>
+    <mergeCell ref="D180:E180"/>
+    <mergeCell ref="D181:E181"/>
+    <mergeCell ref="D182:E182"/>
+    <mergeCell ref="D183:E183"/>
+    <mergeCell ref="D184:E184"/>
+    <mergeCell ref="D185:E185"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A1:E5"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
     <mergeCell ref="D111:E111"/>
     <mergeCell ref="D112:E112"/>
     <mergeCell ref="D95:E95"/>
@@ -3950,96 +5610,16 @@
     <mergeCell ref="D108:E108"/>
     <mergeCell ref="D109:E109"/>
     <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A1:E5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>

<commit_message>
Update sport types define
</commit_message>
<xml_diff>
--- a/files/Sport-UI-Type.xlsx
+++ b/files/Sport-UI-Type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android\Workspace\FitCloudPro-SDK-Android\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android\Workspace\AtGitee\android-sdk-wearkit\FitCloudPro-SDK-Android\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191FEE1E-CA0E-406E-81BC-CD094A152081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AE5EF8-8191-4713-B8DC-9EE0DD0E41CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="843" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="616">
   <si>
     <t>0x04</t>
   </si>
@@ -2143,6 +2143,38 @@
   </si>
   <si>
     <t>0x9B</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0271</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0275</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x9C</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x9D</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>泳池游泳</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>开放水域游泳</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Swimming in pool</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Open-water swim</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -2450,13 +2482,37 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2474,31 +2530,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2807,8 +2839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="I152" sqref="I152"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138:E138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2821,41 +2853,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="29" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
@@ -2867,10 +2899,10 @@
       <c r="C6" s="15" t="s">
         <v>416</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="31" t="s">
         <v>415</v>
       </c>
-      <c r="E6" s="20"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -2882,10 +2914,10 @@
       <c r="C7" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="27" t="s">
         <v>418</v>
       </c>
-      <c r="E7" s="20"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
@@ -2897,10 +2929,10 @@
       <c r="C8" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="27" t="s">
         <v>417</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -2912,10 +2944,10 @@
       <c r="C9" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="27" t="s">
         <v>427</v>
       </c>
-      <c r="E9" s="20"/>
+      <c r="E9" s="28"/>
     </row>
     <row r="10" spans="1:5" ht="25.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -2927,10 +2959,10 @@
       <c r="C10" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="27" t="s">
         <v>429</v>
       </c>
-      <c r="E10" s="20"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -2942,10 +2974,10 @@
       <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="17"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -2957,10 +2989,10 @@
       <c r="C12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -2972,10 +3004,10 @@
       <c r="C13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -2987,10 +3019,10 @@
       <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="17"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -3002,10 +3034,10 @@
       <c r="C15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="17"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -3017,10 +3049,10 @@
       <c r="C16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="17"/>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -3032,10 +3064,10 @@
       <c r="C17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="17"/>
+      <c r="E17" s="23"/>
     </row>
     <row r="18" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -3047,10 +3079,10 @@
       <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="17"/>
+      <c r="E18" s="23"/>
     </row>
     <row r="19" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -3062,10 +3094,10 @@
       <c r="C19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="17"/>
+      <c r="E19" s="23"/>
     </row>
     <row r="20" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -3077,10 +3109,10 @@
       <c r="C20" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="17"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
@@ -3092,10 +3124,10 @@
       <c r="C21" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="17"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
@@ -3107,10 +3139,10 @@
       <c r="C22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="17"/>
+      <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:5" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
@@ -3122,10 +3154,10 @@
       <c r="C23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
@@ -3137,10 +3169,10 @@
       <c r="C24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="17"/>
+      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
@@ -3152,10 +3184,10 @@
       <c r="C25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="17"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -3167,10 +3199,10 @@
       <c r="C26" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="23"/>
     </row>
     <row r="27" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
@@ -3182,10 +3214,10 @@
       <c r="C27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="17"/>
+      <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
@@ -3197,10 +3229,10 @@
       <c r="C28" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E28" s="17"/>
+      <c r="E28" s="23"/>
     </row>
     <row r="29" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
@@ -3212,10 +3244,10 @@
       <c r="C29" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="17"/>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
@@ -3227,10 +3259,10 @@
       <c r="C30" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="17"/>
+      <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -3242,10 +3274,10 @@
       <c r="C31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="17"/>
+      <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
@@ -3257,10 +3289,10 @@
       <c r="C32" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="17"/>
+      <c r="E32" s="23"/>
     </row>
     <row r="33" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -3272,10 +3304,10 @@
       <c r="C33" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="17"/>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
@@ -3287,10 +3319,10 @@
       <c r="C34" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="17"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -3302,10 +3334,10 @@
       <c r="C35" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="23"/>
     </row>
     <row r="36" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
@@ -3317,10 +3349,10 @@
       <c r="C36" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="17"/>
+      <c r="E36" s="23"/>
     </row>
     <row r="37" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -3332,10 +3364,10 @@
       <c r="C37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="E37" s="17"/>
+      <c r="E37" s="23"/>
     </row>
     <row r="38" spans="1:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
@@ -3347,10 +3379,10 @@
       <c r="C38" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="E38" s="17"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
@@ -3362,10 +3394,10 @@
       <c r="C39" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="18"/>
+      <c r="E39" s="32"/>
     </row>
     <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
@@ -3377,10 +3409,10 @@
       <c r="C40" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="18" t="s">
+      <c r="D40" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="18"/>
+      <c r="E40" s="32"/>
     </row>
     <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
@@ -3392,10 +3424,10 @@
       <c r="C41" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="18"/>
+      <c r="E41" s="32"/>
     </row>
     <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
@@ -3407,10 +3439,10 @@
       <c r="C42" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E42" s="18"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
@@ -3422,10 +3454,10 @@
       <c r="C43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="18"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
@@ -3437,10 +3469,10 @@
       <c r="C44" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="18"/>
+      <c r="E44" s="32"/>
     </row>
     <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -3452,10 +3484,10 @@
       <c r="C45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E45" s="18"/>
+      <c r="E45" s="32"/>
     </row>
     <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
@@ -3467,10 +3499,10 @@
       <c r="C46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="E46" s="18"/>
+      <c r="E46" s="32"/>
     </row>
     <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
@@ -3482,10 +3514,10 @@
       <c r="C47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="E47" s="18"/>
+      <c r="E47" s="32"/>
     </row>
     <row r="48" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
@@ -3497,10 +3529,10 @@
       <c r="C48" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D48" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="18"/>
+      <c r="E48" s="32"/>
     </row>
     <row r="49" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
@@ -3512,10 +3544,10 @@
       <c r="C49" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="E49" s="17"/>
+      <c r="E49" s="23"/>
     </row>
     <row r="50" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
@@ -3527,10 +3559,10 @@
       <c r="C50" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="E50" s="17"/>
+      <c r="E50" s="23"/>
     </row>
     <row r="51" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
@@ -3542,10 +3574,10 @@
       <c r="C51" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="E51" s="17"/>
+      <c r="E51" s="23"/>
     </row>
     <row r="52" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
@@ -3557,10 +3589,10 @@
       <c r="C52" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E52" s="17"/>
+      <c r="E52" s="23"/>
     </row>
     <row r="53" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
@@ -3572,10 +3604,10 @@
       <c r="C53" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="E53" s="17"/>
+      <c r="E53" s="23"/>
     </row>
     <row r="54" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
@@ -3587,10 +3619,10 @@
       <c r="C54" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E54" s="17"/>
+      <c r="E54" s="23"/>
     </row>
     <row r="55" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
@@ -3602,10 +3634,10 @@
       <c r="C55" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E55" s="17"/>
+      <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
@@ -3617,10 +3649,10 @@
       <c r="C56" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E56" s="17"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
@@ -3632,10 +3664,10 @@
       <c r="C57" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="17"/>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
@@ -3647,10 +3679,10 @@
       <c r="C58" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E58" s="17"/>
+      <c r="E58" s="23"/>
     </row>
     <row r="59" spans="1:5" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
@@ -3662,10 +3694,10 @@
       <c r="C59" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="17"/>
+      <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
@@ -3677,10 +3709,10 @@
       <c r="C60" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E60" s="17"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
@@ -3692,10 +3724,10 @@
       <c r="C61" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="E61" s="17"/>
+      <c r="E61" s="23"/>
     </row>
     <row r="62" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
@@ -3707,10 +3739,10 @@
       <c r="C62" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="E62" s="17"/>
+      <c r="E62" s="23"/>
     </row>
     <row r="63" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="11" t="s">
@@ -3722,10 +3754,10 @@
       <c r="C63" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E63" s="17"/>
+      <c r="E63" s="23"/>
     </row>
     <row r="64" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="11" t="s">
@@ -3737,10 +3769,10 @@
       <c r="C64" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E64" s="17"/>
+      <c r="E64" s="23"/>
     </row>
     <row r="65" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
@@ -3752,10 +3784,10 @@
       <c r="C65" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="E65" s="17"/>
+      <c r="E65" s="23"/>
     </row>
     <row r="66" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
@@ -3767,10 +3799,10 @@
       <c r="C66" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="17"/>
+      <c r="E66" s="23"/>
     </row>
     <row r="67" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="11" t="s">
@@ -3782,10 +3814,10 @@
       <c r="C67" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="E67" s="17"/>
+      <c r="E67" s="23"/>
     </row>
     <row r="68" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
@@ -3797,10 +3829,10 @@
       <c r="C68" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="E68" s="17"/>
+      <c r="E68" s="23"/>
     </row>
     <row r="69" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
@@ -3812,10 +3844,10 @@
       <c r="C69" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="E69" s="17"/>
+      <c r="E69" s="23"/>
     </row>
     <row r="70" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
@@ -3827,10 +3859,10 @@
       <c r="C70" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E70" s="17"/>
+      <c r="E70" s="23"/>
     </row>
     <row r="71" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11" t="s">
@@ -3842,10 +3874,10 @@
       <c r="C71" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D71" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E71" s="17"/>
+      <c r="E71" s="23"/>
     </row>
     <row r="72" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
@@ -3857,10 +3889,10 @@
       <c r="C72" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="D72" s="16" t="s">
+      <c r="D72" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="E72" s="17"/>
+      <c r="E72" s="23"/>
     </row>
     <row r="73" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
@@ -3872,10 +3904,10 @@
       <c r="C73" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D73" s="16" t="s">
+      <c r="D73" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="E73" s="17"/>
+      <c r="E73" s="23"/>
     </row>
     <row r="74" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
@@ -3887,10 +3919,10 @@
       <c r="C74" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E74" s="17"/>
+      <c r="E74" s="23"/>
     </row>
     <row r="75" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
@@ -3902,10 +3934,10 @@
       <c r="C75" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D75" s="16" t="s">
+      <c r="D75" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E75" s="17"/>
+      <c r="E75" s="23"/>
     </row>
     <row r="76" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
@@ -3917,10 +3949,10 @@
       <c r="C76" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="D76" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="E76" s="17"/>
+      <c r="E76" s="23"/>
     </row>
     <row r="77" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
@@ -3932,10 +3964,10 @@
       <c r="C77" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E77" s="17"/>
+      <c r="E77" s="23"/>
     </row>
     <row r="78" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
@@ -3947,10 +3979,10 @@
       <c r="C78" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D78" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E78" s="17"/>
+      <c r="E78" s="23"/>
     </row>
     <row r="79" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
@@ -3962,10 +3994,10 @@
       <c r="C79" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D79" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E79" s="17"/>
+      <c r="E79" s="23"/>
     </row>
     <row r="80" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
@@ -3977,10 +4009,10 @@
       <c r="C80" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="E80" s="17"/>
+      <c r="E80" s="23"/>
     </row>
     <row r="81" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
@@ -3992,10 +4024,10 @@
       <c r="C81" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="E81" s="17"/>
+      <c r="E81" s="23"/>
     </row>
     <row r="82" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
@@ -4007,10 +4039,10 @@
       <c r="C82" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D82" s="16" t="s">
+      <c r="D82" s="22" t="s">
         <v>216</v>
       </c>
-      <c r="E82" s="17"/>
+      <c r="E82" s="23"/>
     </row>
     <row r="83" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
@@ -4022,10 +4054,10 @@
       <c r="C83" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D83" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="E83" s="17"/>
+      <c r="E83" s="23"/>
     </row>
     <row r="84" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
@@ -4037,10 +4069,10 @@
       <c r="C84" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="D84" s="16" t="s">
+      <c r="D84" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="E84" s="17"/>
+      <c r="E84" s="23"/>
     </row>
     <row r="85" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
@@ -4052,10 +4084,10 @@
       <c r="C85" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="D85" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="E85" s="17"/>
+      <c r="E85" s="23"/>
     </row>
     <row r="86" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
@@ -4067,10 +4099,10 @@
       <c r="C86" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="22" t="s">
         <v>228</v>
       </c>
-      <c r="E86" s="17"/>
+      <c r="E86" s="23"/>
     </row>
     <row r="87" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
@@ -4082,10 +4114,10 @@
       <c r="C87" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E87" s="17"/>
+      <c r="E87" s="23"/>
     </row>
     <row r="88" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
@@ -4097,10 +4129,10 @@
       <c r="C88" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="E88" s="17"/>
+      <c r="E88" s="23"/>
     </row>
     <row r="89" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
@@ -4112,10 +4144,10 @@
       <c r="C89" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="E89" s="17"/>
+      <c r="E89" s="23"/>
     </row>
     <row r="90" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
@@ -4127,10 +4159,10 @@
       <c r="C90" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D90" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="E90" s="17"/>
+      <c r="E90" s="23"/>
     </row>
     <row r="91" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
@@ -4142,10 +4174,10 @@
       <c r="C91" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D91" s="16" t="s">
+      <c r="D91" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="E91" s="17"/>
+      <c r="E91" s="23"/>
     </row>
     <row r="92" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
@@ -4157,10 +4189,10 @@
       <c r="C92" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D92" s="16" t="s">
+      <c r="D92" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="E92" s="17"/>
+      <c r="E92" s="23"/>
     </row>
     <row r="93" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
@@ -4172,10 +4204,10 @@
       <c r="C93" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D93" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="E93" s="17"/>
+      <c r="E93" s="23"/>
     </row>
     <row r="94" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
@@ -4187,10 +4219,10 @@
       <c r="C94" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D94" s="16" t="s">
+      <c r="D94" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="E94" s="17"/>
+      <c r="E94" s="23"/>
     </row>
     <row r="95" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
@@ -4202,10 +4234,10 @@
       <c r="C95" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D95" s="16" t="s">
+      <c r="D95" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="E95" s="17"/>
+      <c r="E95" s="23"/>
     </row>
     <row r="96" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
@@ -4217,10 +4249,10 @@
       <c r="C96" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D96" s="16" t="s">
+      <c r="D96" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="E96" s="17"/>
+      <c r="E96" s="23"/>
     </row>
     <row r="97" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
@@ -4232,10 +4264,10 @@
       <c r="C97" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D97" s="16" t="s">
+      <c r="D97" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="E97" s="17"/>
+      <c r="E97" s="23"/>
     </row>
     <row r="98" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
@@ -4247,10 +4279,10 @@
       <c r="C98" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D98" s="16" t="s">
+      <c r="D98" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="E98" s="17"/>
+      <c r="E98" s="23"/>
     </row>
     <row r="99" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
@@ -4262,10 +4294,10 @@
       <c r="C99" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="D99" s="16" t="s">
+      <c r="D99" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="E99" s="17"/>
+      <c r="E99" s="23"/>
     </row>
     <row r="100" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
@@ -4277,10 +4309,10 @@
       <c r="C100" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="D100" s="16" t="s">
+      <c r="D100" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="E100" s="17"/>
+      <c r="E100" s="23"/>
     </row>
     <row r="101" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
@@ -4292,10 +4324,10 @@
       <c r="C101" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D101" s="16" t="s">
+      <c r="D101" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="E101" s="17"/>
+      <c r="E101" s="23"/>
     </row>
     <row r="102" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
@@ -4307,10 +4339,10 @@
       <c r="C102" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D102" s="16" t="s">
+      <c r="D102" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="E102" s="17"/>
+      <c r="E102" s="23"/>
     </row>
     <row r="103" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="12" t="s">
@@ -4322,10 +4354,10 @@
       <c r="C103" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D103" s="16" t="s">
+      <c r="D103" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E103" s="17"/>
+      <c r="E103" s="23"/>
     </row>
     <row r="104" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="12" t="s">
@@ -4337,10 +4369,10 @@
       <c r="C104" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D104" s="16" t="s">
+      <c r="D104" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="E104" s="17"/>
+      <c r="E104" s="23"/>
     </row>
     <row r="105" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
@@ -4352,10 +4384,10 @@
       <c r="C105" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D105" s="16" t="s">
+      <c r="D105" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E105" s="17"/>
+      <c r="E105" s="23"/>
     </row>
     <row r="106" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
@@ -4367,10 +4399,10 @@
       <c r="C106" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D106" s="16" t="s">
+      <c r="D106" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="E106" s="17"/>
+      <c r="E106" s="23"/>
     </row>
     <row r="107" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
@@ -4382,10 +4414,10 @@
       <c r="C107" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="D107" s="16" t="s">
+      <c r="D107" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E107" s="17"/>
+      <c r="E107" s="23"/>
     </row>
     <row r="108" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
@@ -4397,10 +4429,10 @@
       <c r="C108" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="D108" s="16" t="s">
+      <c r="D108" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E108" s="17"/>
+      <c r="E108" s="23"/>
     </row>
     <row r="109" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="12" t="s">
@@ -4412,10 +4444,10 @@
       <c r="C109" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D109" s="16" t="s">
+      <c r="D109" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E109" s="17"/>
+      <c r="E109" s="23"/>
     </row>
     <row r="110" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="12" t="s">
@@ -4427,10 +4459,10 @@
       <c r="C110" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="D110" s="16" t="s">
+      <c r="D110" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="E110" s="17"/>
+      <c r="E110" s="23"/>
     </row>
     <row r="111" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
@@ -4442,10 +4474,10 @@
       <c r="C111" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D111" s="16" t="s">
+      <c r="D111" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="E111" s="17"/>
+      <c r="E111" s="23"/>
     </row>
     <row r="112" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
@@ -4457,10 +4489,10 @@
       <c r="C112" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="D112" s="16" t="s">
+      <c r="D112" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="E112" s="17"/>
+      <c r="E112" s="23"/>
     </row>
     <row r="113" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
@@ -4472,10 +4504,10 @@
       <c r="C113" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="D113" s="16" t="s">
+      <c r="D113" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="E113" s="17"/>
+      <c r="E113" s="23"/>
     </row>
     <row r="114" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="12" t="s">
@@ -4487,10 +4519,10 @@
       <c r="C114" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D114" s="16" t="s">
+      <c r="D114" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="E114" s="17"/>
+      <c r="E114" s="23"/>
     </row>
     <row r="115" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
@@ -4502,10 +4534,10 @@
       <c r="C115" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D115" s="16" t="s">
+      <c r="D115" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="E115" s="17"/>
+      <c r="E115" s="23"/>
     </row>
     <row r="116" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
@@ -4517,10 +4549,10 @@
       <c r="C116" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="D116" s="16" t="s">
+      <c r="D116" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="E116" s="17"/>
+      <c r="E116" s="23"/>
     </row>
     <row r="117" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="12" t="s">
@@ -4532,10 +4564,10 @@
       <c r="C117" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="D117" s="16" t="s">
+      <c r="D117" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="E117" s="17"/>
+      <c r="E117" s="23"/>
     </row>
     <row r="118" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="12" t="s">
@@ -4547,10 +4579,10 @@
       <c r="C118" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D118" s="16" t="s">
+      <c r="D118" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E118" s="17"/>
+      <c r="E118" s="23"/>
     </row>
     <row r="119" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
@@ -4562,10 +4594,10 @@
       <c r="C119" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D119" s="16" t="s">
+      <c r="D119" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="E119" s="17"/>
+      <c r="E119" s="23"/>
     </row>
     <row r="120" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
@@ -4577,10 +4609,10 @@
       <c r="C120" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="D120" s="16" t="s">
+      <c r="D120" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="E120" s="17"/>
+      <c r="E120" s="23"/>
     </row>
     <row r="121" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
@@ -4592,10 +4624,10 @@
       <c r="C121" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D121" s="16" t="s">
+      <c r="D121" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="E121" s="17"/>
+      <c r="E121" s="23"/>
     </row>
     <row r="122" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="12" t="s">
@@ -4607,901 +4639,946 @@
       <c r="C122" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="D122" s="16" t="s">
+      <c r="D122" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E122" s="17"/>
+      <c r="E122" s="23"/>
     </row>
     <row r="123" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="26" t="s">
+      <c r="A123" s="17" t="s">
         <v>448</v>
       </c>
-      <c r="B123" s="32" t="s">
+      <c r="B123" s="21" t="s">
         <v>449</v>
       </c>
-      <c r="C123" s="32" t="s">
+      <c r="C123" s="21" t="s">
         <v>451</v>
       </c>
-      <c r="D123" s="28" t="s">
+      <c r="D123" s="25" t="s">
         <v>450</v>
       </c>
-      <c r="E123" s="29"/>
+      <c r="E123" s="26"/>
     </row>
     <row r="124" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="26" t="s">
+      <c r="A124" s="17" t="s">
+        <v>614</v>
+      </c>
+      <c r="B124" s="20" t="s">
+        <v>612</v>
+      </c>
+      <c r="C124" s="21" t="s">
+        <v>452</v>
+      </c>
+      <c r="D124" s="25" t="s">
+        <v>453</v>
+      </c>
+      <c r="E124" s="26"/>
+    </row>
+    <row r="125" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="B125" s="20" t="s">
+        <v>613</v>
+      </c>
+      <c r="C125" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="D125" s="25" t="s">
+        <v>459</v>
+      </c>
+      <c r="E125" s="26"/>
+    </row>
+    <row r="126" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="B126" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="C126" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="D126" s="25" t="s">
+        <v>463</v>
+      </c>
+      <c r="E126" s="26"/>
+    </row>
+    <row r="127" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="17" t="s">
+        <v>465</v>
+      </c>
+      <c r="B127" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="D127" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="E127" s="26"/>
+    </row>
+    <row r="128" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="19" t="s">
+        <v>470</v>
+      </c>
+      <c r="B128" s="19" t="s">
+        <v>471</v>
+      </c>
+      <c r="C128" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="D128" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="E128" s="26"/>
+    </row>
+    <row r="129" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="17" t="s">
+        <v>468</v>
+      </c>
+      <c r="B129" s="17" t="s">
+        <v>469</v>
+      </c>
+      <c r="C129" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="D129" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="E129" s="26"/>
+    </row>
+    <row r="130" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="17" t="s">
+        <v>476</v>
+      </c>
+      <c r="B130" s="17" t="s">
+        <v>477</v>
+      </c>
+      <c r="C130" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="D130" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="E130" s="26"/>
+    </row>
+    <row r="131" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="17" t="s">
+        <v>480</v>
+      </c>
+      <c r="B131" s="17" t="s">
+        <v>481</v>
+      </c>
+      <c r="C131" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="D131" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="E131" s="26"/>
+    </row>
+    <row r="132" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="B132" s="17" t="s">
+        <v>487</v>
+      </c>
+      <c r="C132" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="D132" s="25" t="s">
+        <v>577</v>
+      </c>
+      <c r="E132" s="26"/>
+    </row>
+    <row r="133" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="17" t="s">
+        <v>488</v>
+      </c>
+      <c r="B133" s="17" t="s">
+        <v>489</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>484</v>
+      </c>
+      <c r="D133" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="E133" s="26"/>
+    </row>
+    <row r="134" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="17" t="s">
+        <v>491</v>
+      </c>
+      <c r="B134" s="17" t="s">
+        <v>490</v>
+      </c>
+      <c r="C134" s="20" t="s">
+        <v>485</v>
+      </c>
+      <c r="D134" s="25" t="s">
+        <v>579</v>
+      </c>
+      <c r="E134" s="26"/>
+    </row>
+    <row r="135" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="17" t="s">
+        <v>492</v>
+      </c>
+      <c r="B135" s="17" t="s">
+        <v>493</v>
+      </c>
+      <c r="C135" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="D135" s="25" t="s">
+        <v>580</v>
+      </c>
+      <c r="E135" s="26"/>
+    </row>
+    <row r="136" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="C136" s="20" t="s">
+        <v>496</v>
+      </c>
+      <c r="D136" s="25" t="s">
+        <v>581</v>
+      </c>
+      <c r="E136" s="26"/>
+    </row>
+    <row r="137" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="B137" s="17" t="s">
+        <v>499</v>
+      </c>
+      <c r="C137" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="D137" s="25" t="s">
+        <v>582</v>
+      </c>
+      <c r="E137" s="26"/>
+    </row>
+    <row r="138" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="17" t="s">
+        <v>503</v>
+      </c>
+      <c r="B138" s="17" t="s">
+        <v>495</v>
+      </c>
+      <c r="C138" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="D138" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="E138" s="26"/>
+    </row>
+    <row r="139" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="17" t="s">
+        <v>504</v>
+      </c>
+      <c r="B139" s="17" t="s">
+        <v>505</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="D139" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="E139" s="26"/>
+    </row>
+    <row r="140" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="17" t="s">
+        <v>507</v>
+      </c>
+      <c r="B140" s="17" t="s">
+        <v>509</v>
+      </c>
+      <c r="C140" s="20" t="s">
+        <v>508</v>
+      </c>
+      <c r="D140" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="E140" s="26"/>
+    </row>
+    <row r="141" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="17" t="s">
+        <v>512</v>
+      </c>
+      <c r="B141" s="17" t="s">
+        <v>510</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>511</v>
+      </c>
+      <c r="D141" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="E141" s="26"/>
+    </row>
+    <row r="142" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="17" t="s">
+        <v>515</v>
+      </c>
+      <c r="B142" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="C142" s="20" t="s">
+        <v>514</v>
+      </c>
+      <c r="D142" s="25" t="s">
+        <v>587</v>
+      </c>
+      <c r="E142" s="26"/>
+    </row>
+    <row r="143" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="17" t="s">
+        <v>516</v>
+      </c>
+      <c r="B143" s="17" t="s">
+        <v>518</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>520</v>
+      </c>
+      <c r="D143" s="25" t="s">
+        <v>588</v>
+      </c>
+      <c r="E143" s="26"/>
+    </row>
+    <row r="144" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="B144" s="17" t="s">
+        <v>519</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="D144" s="25" t="s">
+        <v>589</v>
+      </c>
+      <c r="E144" s="26"/>
+    </row>
+    <row r="145" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="17" t="s">
+        <v>524</v>
+      </c>
+      <c r="B145" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="C145" s="20" t="s">
+        <v>522</v>
+      </c>
+      <c r="D145" s="25" t="s">
+        <v>590</v>
+      </c>
+      <c r="E145" s="26"/>
+    </row>
+    <row r="146" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>525</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>526</v>
+      </c>
+      <c r="D146" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="E146" s="26"/>
+    </row>
+    <row r="147" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="17" t="s">
+        <v>533</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>528</v>
+      </c>
+      <c r="C147" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="D147" s="25" t="s">
+        <v>592</v>
+      </c>
+      <c r="E147" s="26"/>
+    </row>
+    <row r="148" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="17" t="s">
+        <v>529</v>
+      </c>
+      <c r="B148" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="C148" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="D148" s="25" t="s">
+        <v>593</v>
+      </c>
+      <c r="E148" s="26"/>
+    </row>
+    <row r="149" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="17" t="s">
+        <v>534</v>
+      </c>
+      <c r="B149" s="17" t="s">
+        <v>536</v>
+      </c>
+      <c r="C149" s="20" t="s">
+        <v>535</v>
+      </c>
+      <c r="D149" s="25" t="s">
+        <v>594</v>
+      </c>
+      <c r="E149" s="26"/>
+    </row>
+    <row r="150" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="17" t="s">
+        <v>539</v>
+      </c>
+      <c r="B150" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="C150" s="18" t="s">
+        <v>538</v>
+      </c>
+      <c r="D150" s="25" t="s">
+        <v>595</v>
+      </c>
+      <c r="E150" s="26"/>
+    </row>
+    <row r="151" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="17" t="s">
+        <v>540</v>
+      </c>
+      <c r="B151" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="C151" s="20" t="s">
+        <v>542</v>
+      </c>
+      <c r="D151" s="25" t="s">
+        <v>596</v>
+      </c>
+      <c r="E151" s="26"/>
+    </row>
+    <row r="152" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="B152" s="17" t="s">
+        <v>554</v>
+      </c>
+      <c r="C152" s="20" t="s">
+        <v>543</v>
+      </c>
+      <c r="D152" s="25" t="s">
+        <v>597</v>
+      </c>
+      <c r="E152" s="26"/>
+    </row>
+    <row r="153" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="17" t="s">
+        <v>574</v>
+      </c>
+      <c r="B153" s="17" t="s">
+        <v>555</v>
+      </c>
+      <c r="C153" s="18" t="s">
+        <v>544</v>
+      </c>
+      <c r="D153" s="25" t="s">
+        <v>598</v>
+      </c>
+      <c r="E153" s="26"/>
+    </row>
+    <row r="154" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="17" t="s">
+        <v>573</v>
+      </c>
+      <c r="B154" s="17" t="s">
+        <v>556</v>
+      </c>
+      <c r="C154" s="20" t="s">
+        <v>545</v>
+      </c>
+      <c r="D154" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="E154" s="26"/>
+    </row>
+    <row r="155" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="17" t="s">
+        <v>572</v>
+      </c>
+      <c r="B155" s="17" t="s">
+        <v>557</v>
+      </c>
+      <c r="C155" s="18" t="s">
+        <v>546</v>
+      </c>
+      <c r="D155" s="25" t="s">
+        <v>600</v>
+      </c>
+      <c r="E155" s="26"/>
+    </row>
+    <row r="156" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="17" t="s">
+        <v>571</v>
+      </c>
+      <c r="B156" s="17" t="s">
+        <v>558</v>
+      </c>
+      <c r="C156" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="D156" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="E156" s="26"/>
+    </row>
+    <row r="157" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="17" t="s">
+        <v>570</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>559</v>
+      </c>
+      <c r="C157" s="18" t="s">
+        <v>548</v>
+      </c>
+      <c r="D157" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="E157" s="26"/>
+    </row>
+    <row r="158" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="B158" s="17" t="s">
+        <v>560</v>
+      </c>
+      <c r="C158" s="20" t="s">
+        <v>549</v>
+      </c>
+      <c r="D158" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="E158" s="26"/>
+    </row>
+    <row r="159" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="17" t="s">
+        <v>568</v>
+      </c>
+      <c r="B159" s="17" t="s">
+        <v>561</v>
+      </c>
+      <c r="C159" s="18" t="s">
+        <v>550</v>
+      </c>
+      <c r="D159" s="25" t="s">
+        <v>604</v>
+      </c>
+      <c r="E159" s="26"/>
+    </row>
+    <row r="160" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="B160" s="17" t="s">
+        <v>562</v>
+      </c>
+      <c r="C160" s="20" t="s">
+        <v>551</v>
+      </c>
+      <c r="D160" s="25" t="s">
+        <v>605</v>
+      </c>
+      <c r="E160" s="26"/>
+    </row>
+    <row r="161" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A161" s="17" t="s">
+        <v>566</v>
+      </c>
+      <c r="B161" s="17" t="s">
+        <v>563</v>
+      </c>
+      <c r="C161" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="D161" s="25" t="s">
+        <v>606</v>
+      </c>
+      <c r="E161" s="26"/>
+    </row>
+    <row r="162" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="17" t="s">
+        <v>565</v>
+      </c>
+      <c r="B162" s="17" t="s">
+        <v>564</v>
+      </c>
+      <c r="C162" s="20" t="s">
+        <v>553</v>
+      </c>
+      <c r="D162" s="25" t="s">
+        <v>607</v>
+      </c>
+      <c r="E162" s="26"/>
+    </row>
+    <row r="163" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A163" s="17" t="s">
         <v>455</v>
       </c>
-      <c r="B124" s="32" t="s">
+      <c r="B163" s="21" t="s">
         <v>454</v>
       </c>
-      <c r="C124" s="32" t="s">
-        <v>452</v>
-      </c>
-      <c r="D124" s="28" t="s">
-        <v>453</v>
-      </c>
-      <c r="E124" s="29"/>
-    </row>
-    <row r="125" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="26" t="s">
+      <c r="C163" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="D163" s="25" t="s">
+        <v>610</v>
+      </c>
+      <c r="E163" s="26"/>
+    </row>
+    <row r="164" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A164" s="17" t="s">
         <v>456</v>
       </c>
-      <c r="B125" s="32" t="s">
+      <c r="B164" s="21" t="s">
         <v>457</v>
       </c>
-      <c r="C125" s="32" t="s">
-        <v>458</v>
-      </c>
-      <c r="D125" s="28" t="s">
-        <v>459</v>
-      </c>
-      <c r="E125" s="29"/>
-    </row>
-    <row r="126" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="26" t="s">
-        <v>461</v>
-      </c>
-      <c r="B126" s="32" t="s">
-        <v>460</v>
-      </c>
-      <c r="C126" s="32" t="s">
-        <v>462</v>
-      </c>
-      <c r="D126" s="28" t="s">
-        <v>463</v>
-      </c>
-      <c r="E126" s="29"/>
-    </row>
-    <row r="127" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="26" t="s">
-        <v>465</v>
-      </c>
-      <c r="B127" s="32" t="s">
-        <v>464</v>
-      </c>
-      <c r="C127" s="32" t="s">
-        <v>466</v>
-      </c>
-      <c r="D127" s="28" t="s">
-        <v>467</v>
-      </c>
-      <c r="E127" s="29"/>
-    </row>
-    <row r="128" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="30" t="s">
-        <v>470</v>
-      </c>
-      <c r="B128" s="30" t="s">
-        <v>471</v>
-      </c>
-      <c r="C128" s="31" t="s">
-        <v>472</v>
-      </c>
-      <c r="D128" s="28" t="s">
-        <v>474</v>
-      </c>
-      <c r="E128" s="29"/>
-    </row>
-    <row r="129" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="26" t="s">
-        <v>468</v>
-      </c>
-      <c r="B129" s="26" t="s">
-        <v>469</v>
-      </c>
-      <c r="C129" s="27" t="s">
-        <v>473</v>
-      </c>
-      <c r="D129" s="28" t="s">
-        <v>475</v>
-      </c>
-      <c r="E129" s="29"/>
-    </row>
-    <row r="130" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="26" t="s">
-        <v>476</v>
-      </c>
-      <c r="B130" s="26" t="s">
-        <v>477</v>
-      </c>
-      <c r="C130" s="31" t="s">
-        <v>478</v>
-      </c>
-      <c r="D130" s="28" t="s">
-        <v>479</v>
-      </c>
-      <c r="E130" s="29"/>
-    </row>
-    <row r="131" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="26" t="s">
-        <v>480</v>
-      </c>
-      <c r="B131" s="26" t="s">
-        <v>481</v>
-      </c>
-      <c r="C131" s="31" t="s">
-        <v>482</v>
-      </c>
-      <c r="D131" s="28" t="s">
-        <v>576</v>
-      </c>
-      <c r="E131" s="29"/>
-    </row>
-    <row r="132" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="26" t="s">
-        <v>486</v>
-      </c>
-      <c r="B132" s="26" t="s">
-        <v>487</v>
-      </c>
-      <c r="C132" s="27" t="s">
-        <v>483</v>
-      </c>
-      <c r="D132" s="28" t="s">
-        <v>577</v>
-      </c>
-      <c r="E132" s="29"/>
-    </row>
-    <row r="133" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="26" t="s">
-        <v>488</v>
-      </c>
-      <c r="B133" s="26" t="s">
-        <v>489</v>
-      </c>
-      <c r="C133" s="31" t="s">
-        <v>484</v>
-      </c>
-      <c r="D133" s="28" t="s">
-        <v>578</v>
-      </c>
-      <c r="E133" s="29"/>
-    </row>
-    <row r="134" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="26" t="s">
-        <v>491</v>
-      </c>
-      <c r="B134" s="26" t="s">
-        <v>490</v>
-      </c>
-      <c r="C134" s="31" t="s">
-        <v>485</v>
-      </c>
-      <c r="D134" s="28" t="s">
-        <v>579</v>
-      </c>
-      <c r="E134" s="29"/>
-    </row>
-    <row r="135" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="B135" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="C135" s="27" t="s">
-        <v>494</v>
-      </c>
-      <c r="D135" s="28" t="s">
-        <v>580</v>
-      </c>
-      <c r="E135" s="29"/>
-    </row>
-    <row r="136" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="26" t="s">
-        <v>498</v>
-      </c>
-      <c r="B136" s="26" t="s">
-        <v>497</v>
-      </c>
-      <c r="C136" s="31" t="s">
-        <v>496</v>
-      </c>
-      <c r="D136" s="28" t="s">
-        <v>581</v>
-      </c>
-      <c r="E136" s="29"/>
-    </row>
-    <row r="137" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="26" t="s">
-        <v>501</v>
-      </c>
-      <c r="B137" s="26" t="s">
-        <v>499</v>
-      </c>
-      <c r="C137" s="31" t="s">
-        <v>500</v>
-      </c>
-      <c r="D137" s="28" t="s">
-        <v>582</v>
-      </c>
-      <c r="E137" s="29"/>
-    </row>
-    <row r="138" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="26" t="s">
-        <v>503</v>
-      </c>
-      <c r="B138" s="26" t="s">
-        <v>495</v>
-      </c>
-      <c r="C138" s="27" t="s">
-        <v>502</v>
-      </c>
-      <c r="D138" s="28" t="s">
-        <v>583</v>
-      </c>
-      <c r="E138" s="29"/>
-    </row>
-    <row r="139" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="26" t="s">
-        <v>504</v>
-      </c>
-      <c r="B139" s="26" t="s">
-        <v>505</v>
-      </c>
-      <c r="C139" s="31" t="s">
-        <v>506</v>
-      </c>
-      <c r="D139" s="28" t="s">
-        <v>584</v>
-      </c>
-      <c r="E139" s="29"/>
-    </row>
-    <row r="140" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="26" t="s">
-        <v>507</v>
-      </c>
-      <c r="B140" s="26" t="s">
-        <v>509</v>
-      </c>
-      <c r="C140" s="31" t="s">
-        <v>508</v>
-      </c>
-      <c r="D140" s="28" t="s">
-        <v>585</v>
-      </c>
-      <c r="E140" s="29"/>
-    </row>
-    <row r="141" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="26" t="s">
-        <v>512</v>
-      </c>
-      <c r="B141" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="C141" s="27" t="s">
-        <v>511</v>
-      </c>
-      <c r="D141" s="28" t="s">
-        <v>586</v>
-      </c>
-      <c r="E141" s="29"/>
-    </row>
-    <row r="142" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="26" t="s">
-        <v>515</v>
-      </c>
-      <c r="B142" s="26" t="s">
-        <v>513</v>
-      </c>
-      <c r="C142" s="31" t="s">
-        <v>514</v>
-      </c>
-      <c r="D142" s="28" t="s">
-        <v>587</v>
-      </c>
-      <c r="E142" s="29"/>
-    </row>
-    <row r="143" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="26" t="s">
-        <v>516</v>
-      </c>
-      <c r="B143" s="26" t="s">
-        <v>518</v>
-      </c>
-      <c r="C143" s="31" t="s">
-        <v>520</v>
-      </c>
-      <c r="D143" s="28" t="s">
-        <v>588</v>
-      </c>
-      <c r="E143" s="29"/>
-    </row>
-    <row r="144" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="26" t="s">
-        <v>517</v>
-      </c>
-      <c r="B144" s="26" t="s">
-        <v>519</v>
-      </c>
-      <c r="C144" s="27" t="s">
-        <v>521</v>
-      </c>
-      <c r="D144" s="28" t="s">
-        <v>589</v>
-      </c>
-      <c r="E144" s="29"/>
-    </row>
-    <row r="145" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="26" t="s">
-        <v>524</v>
-      </c>
-      <c r="B145" s="26" t="s">
-        <v>523</v>
-      </c>
-      <c r="C145" s="31" t="s">
-        <v>522</v>
-      </c>
-      <c r="D145" s="28" t="s">
-        <v>590</v>
-      </c>
-      <c r="E145" s="29"/>
-    </row>
-    <row r="146" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="26" t="s">
-        <v>527</v>
-      </c>
-      <c r="B146" s="26" t="s">
-        <v>525</v>
-      </c>
-      <c r="C146" s="31" t="s">
-        <v>526</v>
-      </c>
-      <c r="D146" s="28" t="s">
-        <v>591</v>
-      </c>
-      <c r="E146" s="29"/>
-    </row>
-    <row r="147" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="26" t="s">
-        <v>533</v>
-      </c>
-      <c r="B147" s="26" t="s">
-        <v>528</v>
-      </c>
-      <c r="C147" s="27" t="s">
-        <v>532</v>
-      </c>
-      <c r="D147" s="28" t="s">
-        <v>592</v>
-      </c>
-      <c r="E147" s="29"/>
-    </row>
-    <row r="148" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="26" t="s">
-        <v>529</v>
-      </c>
-      <c r="B148" s="26" t="s">
-        <v>530</v>
-      </c>
-      <c r="C148" s="31" t="s">
-        <v>531</v>
-      </c>
-      <c r="D148" s="28" t="s">
-        <v>593</v>
-      </c>
-      <c r="E148" s="29"/>
-    </row>
-    <row r="149" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="26" t="s">
-        <v>534</v>
-      </c>
-      <c r="B149" s="26" t="s">
-        <v>536</v>
-      </c>
-      <c r="C149" s="31" t="s">
-        <v>535</v>
-      </c>
-      <c r="D149" s="28" t="s">
-        <v>594</v>
-      </c>
-      <c r="E149" s="29"/>
-    </row>
-    <row r="150" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="26" t="s">
-        <v>539</v>
-      </c>
-      <c r="B150" s="26" t="s">
-        <v>537</v>
-      </c>
-      <c r="C150" s="27" t="s">
-        <v>538</v>
-      </c>
-      <c r="D150" s="28" t="s">
-        <v>595</v>
-      </c>
-      <c r="E150" s="29"/>
-    </row>
-    <row r="151" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="26" t="s">
-        <v>540</v>
-      </c>
-      <c r="B151" s="26" t="s">
-        <v>541</v>
-      </c>
-      <c r="C151" s="31" t="s">
-        <v>542</v>
-      </c>
-      <c r="D151" s="28" t="s">
-        <v>596</v>
-      </c>
-      <c r="E151" s="29"/>
-    </row>
-    <row r="152" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="26" t="s">
-        <v>575</v>
-      </c>
-      <c r="B152" s="26" t="s">
-        <v>554</v>
-      </c>
-      <c r="C152" s="31" t="s">
-        <v>543</v>
-      </c>
-      <c r="D152" s="28" t="s">
-        <v>597</v>
-      </c>
-      <c r="E152" s="29"/>
-    </row>
-    <row r="153" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="26" t="s">
-        <v>574</v>
-      </c>
-      <c r="B153" s="26" t="s">
-        <v>555</v>
-      </c>
-      <c r="C153" s="27" t="s">
-        <v>544</v>
-      </c>
-      <c r="D153" s="28" t="s">
-        <v>598</v>
-      </c>
-      <c r="E153" s="29"/>
-    </row>
-    <row r="154" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="26" t="s">
-        <v>573</v>
-      </c>
-      <c r="B154" s="26" t="s">
-        <v>556</v>
-      </c>
-      <c r="C154" s="31" t="s">
-        <v>545</v>
-      </c>
-      <c r="D154" s="28" t="s">
-        <v>599</v>
-      </c>
-      <c r="E154" s="29"/>
-    </row>
-    <row r="155" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="26" t="s">
-        <v>572</v>
-      </c>
-      <c r="B155" s="26" t="s">
-        <v>557</v>
-      </c>
-      <c r="C155" s="27" t="s">
-        <v>546</v>
-      </c>
-      <c r="D155" s="28" t="s">
-        <v>600</v>
-      </c>
-      <c r="E155" s="29"/>
-    </row>
-    <row r="156" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="26" t="s">
-        <v>571</v>
-      </c>
-      <c r="B156" s="26" t="s">
-        <v>558</v>
-      </c>
-      <c r="C156" s="31" t="s">
-        <v>547</v>
-      </c>
-      <c r="D156" s="28" t="s">
-        <v>601</v>
-      </c>
-      <c r="E156" s="29"/>
-    </row>
-    <row r="157" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="26" t="s">
-        <v>570</v>
-      </c>
-      <c r="B157" s="26" t="s">
-        <v>559</v>
-      </c>
-      <c r="C157" s="27" t="s">
-        <v>548</v>
-      </c>
-      <c r="D157" s="28" t="s">
-        <v>602</v>
-      </c>
-      <c r="E157" s="29"/>
-    </row>
-    <row r="158" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="26" t="s">
-        <v>569</v>
-      </c>
-      <c r="B158" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="C158" s="31" t="s">
-        <v>549</v>
-      </c>
-      <c r="D158" s="28" t="s">
-        <v>603</v>
-      </c>
-      <c r="E158" s="29"/>
-    </row>
-    <row r="159" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="26" t="s">
-        <v>568</v>
-      </c>
-      <c r="B159" s="26" t="s">
-        <v>561</v>
-      </c>
-      <c r="C159" s="27" t="s">
-        <v>550</v>
-      </c>
-      <c r="D159" s="28" t="s">
-        <v>604</v>
-      </c>
-      <c r="E159" s="29"/>
-    </row>
-    <row r="160" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="26" t="s">
-        <v>567</v>
-      </c>
-      <c r="B160" s="26" t="s">
-        <v>562</v>
-      </c>
-      <c r="C160" s="31" t="s">
-        <v>551</v>
-      </c>
-      <c r="D160" s="28" t="s">
-        <v>605</v>
-      </c>
-      <c r="E160" s="29"/>
-    </row>
-    <row r="161" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="26" t="s">
-        <v>566</v>
-      </c>
-      <c r="B161" s="26" t="s">
-        <v>563</v>
-      </c>
-      <c r="C161" s="27" t="s">
-        <v>552</v>
-      </c>
-      <c r="D161" s="28" t="s">
-        <v>606</v>
-      </c>
-      <c r="E161" s="29"/>
-    </row>
-    <row r="162" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="26" t="s">
-        <v>565</v>
-      </c>
-      <c r="B162" s="26" t="s">
-        <v>564</v>
-      </c>
-      <c r="C162" s="31" t="s">
-        <v>553</v>
-      </c>
-      <c r="D162" s="28" t="s">
-        <v>607</v>
-      </c>
-      <c r="E162" s="29"/>
-    </row>
-    <row r="163" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="12"/>
-      <c r="B163" s="13"/>
-      <c r="C163" s="25"/>
-      <c r="D163" s="24"/>
-      <c r="E163" s="17"/>
-    </row>
-    <row r="164" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="12"/>
-      <c r="B164" s="13"/>
-      <c r="C164" s="1"/>
-      <c r="D164" s="16"/>
-      <c r="E164" s="17"/>
+      <c r="C164" s="20" t="s">
+        <v>609</v>
+      </c>
+      <c r="D164" s="25" t="s">
+        <v>611</v>
+      </c>
+      <c r="E164" s="26"/>
     </row>
     <row r="165" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="12"/>
       <c r="B165" s="13"/>
-      <c r="C165" s="25"/>
+      <c r="C165" s="16"/>
       <c r="D165" s="24"/>
-      <c r="E165" s="17"/>
+      <c r="E165" s="23"/>
     </row>
     <row r="166" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="12"/>
       <c r="B166" s="13"/>
       <c r="C166" s="1"/>
-      <c r="D166" s="16"/>
-      <c r="E166" s="17"/>
+      <c r="D166" s="22"/>
+      <c r="E166" s="23"/>
     </row>
     <row r="167" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="12"/>
       <c r="B167" s="13"/>
-      <c r="C167" s="25"/>
+      <c r="C167" s="16"/>
       <c r="D167" s="24"/>
-      <c r="E167" s="17"/>
+      <c r="E167" s="23"/>
     </row>
     <row r="168" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="12"/>
       <c r="B168" s="13"/>
       <c r="C168" s="1"/>
-      <c r="D168" s="16"/>
-      <c r="E168" s="17"/>
+      <c r="D168" s="22"/>
+      <c r="E168" s="23"/>
     </row>
     <row r="169" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="12"/>
       <c r="B169" s="13"/>
-      <c r="C169" s="25"/>
+      <c r="C169" s="16"/>
       <c r="D169" s="24"/>
-      <c r="E169" s="17"/>
+      <c r="E169" s="23"/>
     </row>
     <row r="170" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="12"/>
       <c r="B170" s="13"/>
       <c r="C170" s="1"/>
-      <c r="D170" s="16"/>
-      <c r="E170" s="17"/>
+      <c r="D170" s="22"/>
+      <c r="E170" s="23"/>
     </row>
     <row r="171" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="12"/>
       <c r="B171" s="13"/>
-      <c r="C171" s="25"/>
+      <c r="C171" s="16"/>
       <c r="D171" s="24"/>
-      <c r="E171" s="17"/>
+      <c r="E171" s="23"/>
     </row>
     <row r="172" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="12"/>
       <c r="B172" s="13"/>
       <c r="C172" s="1"/>
-      <c r="D172" s="16"/>
-      <c r="E172" s="17"/>
+      <c r="D172" s="22"/>
+      <c r="E172" s="23"/>
     </row>
     <row r="173" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="12"/>
       <c r="B173" s="13"/>
-      <c r="C173" s="25"/>
+      <c r="C173" s="16"/>
       <c r="D173" s="24"/>
-      <c r="E173" s="17"/>
+      <c r="E173" s="23"/>
     </row>
     <row r="174" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="B174" s="13"/>
       <c r="C174" s="1"/>
-      <c r="D174" s="16"/>
-      <c r="E174" s="17"/>
+      <c r="D174" s="22"/>
+      <c r="E174" s="23"/>
     </row>
     <row r="175" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="12"/>
       <c r="B175" s="13"/>
-      <c r="C175" s="25"/>
+      <c r="C175" s="16"/>
       <c r="D175" s="24"/>
-      <c r="E175" s="17"/>
+      <c r="E175" s="23"/>
     </row>
     <row r="176" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="12"/>
       <c r="B176" s="13"/>
       <c r="C176" s="1"/>
-      <c r="D176" s="16"/>
-      <c r="E176" s="17"/>
+      <c r="D176" s="22"/>
+      <c r="E176" s="23"/>
     </row>
     <row r="177" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="12"/>
       <c r="B177" s="13"/>
-      <c r="C177" s="25"/>
+      <c r="C177" s="16"/>
       <c r="D177" s="24"/>
-      <c r="E177" s="17"/>
+      <c r="E177" s="23"/>
     </row>
     <row r="178" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="12"/>
       <c r="B178" s="13"/>
       <c r="C178" s="1"/>
-      <c r="D178" s="16"/>
-      <c r="E178" s="17"/>
+      <c r="D178" s="22"/>
+      <c r="E178" s="23"/>
     </row>
     <row r="179" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="12"/>
       <c r="B179" s="13"/>
-      <c r="C179" s="25"/>
+      <c r="C179" s="16"/>
       <c r="D179" s="24"/>
-      <c r="E179" s="17"/>
+      <c r="E179" s="23"/>
     </row>
     <row r="180" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A180" s="12"/>
       <c r="B180" s="13"/>
       <c r="C180" s="1"/>
-      <c r="D180" s="16"/>
-      <c r="E180" s="17"/>
+      <c r="D180" s="22"/>
+      <c r="E180" s="23"/>
     </row>
     <row r="181" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="12"/>
       <c r="B181" s="13"/>
-      <c r="C181" s="25"/>
+      <c r="C181" s="16"/>
       <c r="D181" s="24"/>
-      <c r="E181" s="17"/>
+      <c r="E181" s="23"/>
     </row>
     <row r="182" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="12"/>
       <c r="B182" s="13"/>
       <c r="C182" s="1"/>
-      <c r="D182" s="16"/>
-      <c r="E182" s="17"/>
+      <c r="D182" s="22"/>
+      <c r="E182" s="23"/>
     </row>
     <row r="183" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="12"/>
       <c r="B183" s="13"/>
-      <c r="C183" s="25"/>
+      <c r="C183" s="16"/>
       <c r="D183" s="24"/>
-      <c r="E183" s="17"/>
+      <c r="E183" s="23"/>
     </row>
     <row r="184" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="12"/>
       <c r="B184" s="13"/>
       <c r="C184" s="1"/>
-      <c r="D184" s="16"/>
-      <c r="E184" s="17"/>
+      <c r="D184" s="22"/>
+      <c r="E184" s="23"/>
     </row>
     <row r="185" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A185" s="12"/>
       <c r="B185" s="13"/>
-      <c r="C185" s="25"/>
+      <c r="C185" s="16"/>
       <c r="D185" s="24"/>
-      <c r="E185" s="17"/>
+      <c r="E185" s="23"/>
     </row>
     <row r="186" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="12"/>
       <c r="B186" s="13"/>
       <c r="C186" s="1"/>
-      <c r="D186" s="16"/>
-      <c r="E186" s="17"/>
+      <c r="D186" s="22"/>
+      <c r="E186" s="23"/>
     </row>
     <row r="187" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="12"/>
       <c r="B187" s="13"/>
-      <c r="C187" s="25"/>
+      <c r="C187" s="16"/>
       <c r="D187" s="24"/>
-      <c r="E187" s="17"/>
+      <c r="E187" s="23"/>
     </row>
     <row r="188" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="12"/>
       <c r="B188" s="13"/>
       <c r="C188" s="1"/>
-      <c r="D188" s="16"/>
-      <c r="E188" s="17"/>
+      <c r="D188" s="22"/>
+      <c r="E188" s="23"/>
     </row>
     <row r="189" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="12"/>
       <c r="B189" s="13"/>
-      <c r="C189" s="25"/>
+      <c r="C189" s="16"/>
       <c r="D189" s="24"/>
-      <c r="E189" s="17"/>
+      <c r="E189" s="23"/>
     </row>
     <row r="190" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="B190" s="13"/>
       <c r="C190" s="1"/>
-      <c r="D190" s="16"/>
-      <c r="E190" s="17"/>
+      <c r="D190" s="22"/>
+      <c r="E190" s="23"/>
     </row>
     <row r="191" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="12"/>
       <c r="B191" s="13"/>
-      <c r="C191" s="25"/>
+      <c r="C191" s="16"/>
       <c r="D191" s="24"/>
-      <c r="E191" s="17"/>
+      <c r="E191" s="23"/>
     </row>
     <row r="192" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="12"/>
       <c r="B192" s="13"/>
       <c r="C192" s="1"/>
-      <c r="D192" s="16"/>
-      <c r="E192" s="17"/>
+      <c r="D192" s="22"/>
+      <c r="E192" s="23"/>
     </row>
     <row r="193" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
       <c r="B193" s="13"/>
-      <c r="C193" s="25"/>
+      <c r="C193" s="16"/>
       <c r="D193" s="24"/>
-      <c r="E193" s="17"/>
+      <c r="E193" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="189">
-    <mergeCell ref="D186:E186"/>
-    <mergeCell ref="D187:E187"/>
-    <mergeCell ref="D188:E188"/>
-    <mergeCell ref="D189:E189"/>
-    <mergeCell ref="D190:E190"/>
-    <mergeCell ref="D191:E191"/>
-    <mergeCell ref="D192:E192"/>
-    <mergeCell ref="D193:E193"/>
-    <mergeCell ref="D177:E177"/>
-    <mergeCell ref="D178:E178"/>
-    <mergeCell ref="D179:E179"/>
-    <mergeCell ref="D180:E180"/>
-    <mergeCell ref="D181:E181"/>
-    <mergeCell ref="D182:E182"/>
-    <mergeCell ref="D183:E183"/>
-    <mergeCell ref="D184:E184"/>
-    <mergeCell ref="D185:E185"/>
-    <mergeCell ref="D168:E168"/>
-    <mergeCell ref="D169:E169"/>
-    <mergeCell ref="D170:E170"/>
-    <mergeCell ref="D171:E171"/>
-    <mergeCell ref="D172:E172"/>
-    <mergeCell ref="D173:E173"/>
-    <mergeCell ref="D174:E174"/>
-    <mergeCell ref="D175:E175"/>
-    <mergeCell ref="D176:E176"/>
-    <mergeCell ref="D159:E159"/>
-    <mergeCell ref="D160:E160"/>
-    <mergeCell ref="D161:E161"/>
-    <mergeCell ref="D162:E162"/>
-    <mergeCell ref="D163:E163"/>
-    <mergeCell ref="D164:E164"/>
-    <mergeCell ref="D165:E165"/>
-    <mergeCell ref="D166:E166"/>
-    <mergeCell ref="D167:E167"/>
-    <mergeCell ref="D150:E150"/>
-    <mergeCell ref="D151:E151"/>
-    <mergeCell ref="D152:E152"/>
-    <mergeCell ref="D153:E153"/>
-    <mergeCell ref="D154:E154"/>
-    <mergeCell ref="D155:E155"/>
-    <mergeCell ref="D156:E156"/>
-    <mergeCell ref="D157:E157"/>
-    <mergeCell ref="D158:E158"/>
-    <mergeCell ref="D141:E141"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="D143:E143"/>
-    <mergeCell ref="D144:E144"/>
-    <mergeCell ref="D145:E145"/>
-    <mergeCell ref="D146:E146"/>
-    <mergeCell ref="D147:E147"/>
-    <mergeCell ref="D148:E148"/>
-    <mergeCell ref="D149:E149"/>
-    <mergeCell ref="D132:E132"/>
-    <mergeCell ref="D133:E133"/>
-    <mergeCell ref="D134:E134"/>
-    <mergeCell ref="D135:E135"/>
-    <mergeCell ref="D136:E136"/>
-    <mergeCell ref="D137:E137"/>
-    <mergeCell ref="D138:E138"/>
-    <mergeCell ref="D139:E139"/>
-    <mergeCell ref="D140:E140"/>
-    <mergeCell ref="D123:E123"/>
-    <mergeCell ref="D124:E124"/>
-    <mergeCell ref="D125:E125"/>
-    <mergeCell ref="D126:E126"/>
-    <mergeCell ref="D127:E127"/>
-    <mergeCell ref="D128:E128"/>
-    <mergeCell ref="D129:E129"/>
-    <mergeCell ref="D130:E130"/>
-    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D122:E122"/>
+    <mergeCell ref="D113:E113"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="D20:E20"/>
@@ -5520,106 +5597,77 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D122:E122"/>
-    <mergeCell ref="D113:E113"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="D118:E118"/>
-    <mergeCell ref="D119:E119"/>
-    <mergeCell ref="D120:E120"/>
-    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="D123:E123"/>
+    <mergeCell ref="D124:E124"/>
+    <mergeCell ref="D125:E125"/>
+    <mergeCell ref="D126:E126"/>
+    <mergeCell ref="D127:E127"/>
+    <mergeCell ref="D128:E128"/>
+    <mergeCell ref="D129:E129"/>
+    <mergeCell ref="D130:E130"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="D135:E135"/>
+    <mergeCell ref="D136:E136"/>
+    <mergeCell ref="D137:E137"/>
+    <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D139:E139"/>
+    <mergeCell ref="D140:E140"/>
+    <mergeCell ref="D141:E141"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="D143:E143"/>
+    <mergeCell ref="D144:E144"/>
+    <mergeCell ref="D145:E145"/>
+    <mergeCell ref="D146:E146"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="D150:E150"/>
+    <mergeCell ref="D151:E151"/>
+    <mergeCell ref="D152:E152"/>
+    <mergeCell ref="D153:E153"/>
+    <mergeCell ref="D154:E154"/>
+    <mergeCell ref="D155:E155"/>
+    <mergeCell ref="D156:E156"/>
+    <mergeCell ref="D157:E157"/>
+    <mergeCell ref="D158:E158"/>
+    <mergeCell ref="D159:E159"/>
+    <mergeCell ref="D160:E160"/>
+    <mergeCell ref="D161:E161"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="D165:E165"/>
+    <mergeCell ref="D166:E166"/>
+    <mergeCell ref="D167:E167"/>
+    <mergeCell ref="D168:E168"/>
+    <mergeCell ref="D169:E169"/>
+    <mergeCell ref="D170:E170"/>
+    <mergeCell ref="D171:E171"/>
+    <mergeCell ref="D172:E172"/>
+    <mergeCell ref="D173:E173"/>
+    <mergeCell ref="D174:E174"/>
+    <mergeCell ref="D175:E175"/>
+    <mergeCell ref="D176:E176"/>
+    <mergeCell ref="D186:E186"/>
+    <mergeCell ref="D187:E187"/>
+    <mergeCell ref="D188:E188"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="D190:E190"/>
+    <mergeCell ref="D191:E191"/>
+    <mergeCell ref="D192:E192"/>
+    <mergeCell ref="D193:E193"/>
+    <mergeCell ref="D177:E177"/>
+    <mergeCell ref="D178:E178"/>
+    <mergeCell ref="D179:E179"/>
+    <mergeCell ref="D180:E180"/>
+    <mergeCell ref="D181:E181"/>
+    <mergeCell ref="D182:E182"/>
+    <mergeCell ref="D183:E183"/>
+    <mergeCell ref="D184:E184"/>
+    <mergeCell ref="D185:E185"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>

</xml_diff>